<commit_message>
YF23A-6 add EFM code template
</commit_message>
<xml_diff>
--- a/Docs/aerodata.xlsx
+++ b/Docs/aerodata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Saved Games\DCS\Mods\aircraft\YF-23A Black Widow\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DEF970BF-A098-44B0-9A67-60C289AE9BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1B9A76C-2445-4F44-A25A-94C9100D5721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6C4CA6DD-015D-4D4D-AF65-FC962CCBE673}"/>
   </bookViews>
@@ -3027,58 +3027,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="117"/>
                 <c:pt idx="99">
-                  <c:v>1.6500000000000001E-2</c:v>
+                  <c:v>1.6299999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>1.6500000000000001E-2</c:v>
+                  <c:v>1.6299999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>1.6500000000000001E-2</c:v>
+                  <c:v>1.6299999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>1.7500000000000002E-2</c:v>
+                  <c:v>1.7000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>0.02</c:v>
+                  <c:v>1.7000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>0.02</c:v>
+                  <c:v>1.7999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>1.84E-2</c:v>
+                  <c:v>2.1999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>1.7999999999999999E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>1.9E-2</c:v>
+                  <c:v>4.2999999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>2.1000000000000001E-2</c:v>
+                  <c:v>4.4999999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>2.1000000000000001E-2</c:v>
+                  <c:v>4.3999999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>2.0500000000000001E-2</c:v>
+                  <c:v>4.2999999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>1.9E-2</c:v>
+                  <c:v>4.2000000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>1.8599999999999998E-2</c:v>
+                  <c:v>4.2000000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>1.8599999999999998E-2</c:v>
+                  <c:v>4.1000000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>1.8599999999999998E-2</c:v>
+                  <c:v>4.1000000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>1.7999999999999999E-2</c:v>
+                  <c:v>3.9E-2</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>2.1999999999999999E-2</c:v>
+                  <c:v>3.7999999999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6174,58 +6174,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="117"/>
                 <c:pt idx="99">
-                  <c:v>5.5E-2</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>5.5E-2</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>5.5E-2</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>5.5E-2</c:v>
+                  <c:v>7.2999999999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>5.5E-2</c:v>
+                  <c:v>7.5999999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>5.5E-2</c:v>
+                  <c:v>7.9000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>5.8000000000000003E-2</c:v>
+                  <c:v>8.3000000000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>6.2E-2</c:v>
+                  <c:v>8.5000000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>6.2E-2</c:v>
+                  <c:v>8.5999999999999993E-2</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>6.2E-2</c:v>
+                  <c:v>8.3000000000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>0.06</c:v>
+                  <c:v>7.6999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>5.6000000000000001E-2</c:v>
+                  <c:v>6.9500000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>5.1999999999999998E-2</c:v>
+                  <c:v>5.7000000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>4.2000000000000003E-2</c:v>
+                  <c:v>4.7E-2</c:v>
                 </c:pt>
                 <c:pt idx="113">
                   <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>3.6999999999999998E-2</c:v>
+                  <c:v>3.5000000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="115">
                   <c:v>3.3000000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>2.3E-2</c:v>
+                  <c:v>3.3000000000000002E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9303,28 +9303,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="117"/>
                 <c:pt idx="99">
-                  <c:v>0.19800000000000001</c:v>
+                  <c:v>0.13400000000000001</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.19800000000000001</c:v>
+                  <c:v>0.13400000000000001</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>0.19800000000000001</c:v>
+                  <c:v>0.13400000000000001</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>0.19800000000000001</c:v>
+                  <c:v>0.128</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>0.19800000000000001</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>0.19800000000000001</c:v>
+                  <c:v>0.123</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>0.19800000000000001</c:v>
+                  <c:v>0.155</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>0.19800000000000001</c:v>
+                  <c:v>0.18</c:v>
                 </c:pt>
                 <c:pt idx="107">
                   <c:v>0.20100000000000001</c:v>
@@ -12450,37 +12450,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="117"/>
                 <c:pt idx="99">
-                  <c:v>0.22</c:v>
+                  <c:v>4.2000000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.22</c:v>
+                  <c:v>4.2000000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>0.22</c:v>
+                  <c:v>4.2000000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>0.28000000000000003</c:v>
+                  <c:v>4.8000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>0.28000000000000003</c:v>
+                  <c:v>4.8000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>0.28000000000000003</c:v>
+                  <c:v>4.8000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>0.2</c:v>
+                  <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>0.15</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="107">
                   <c:v>0.09</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>0.08</c:v>
+                  <c:v>0.09</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>0.1</c:v>
+                  <c:v>0.96</c:v>
                 </c:pt>
                 <c:pt idx="110">
                   <c:v>0.13600000000000001</c:v>
@@ -12489,16 +12489,16 @@
                   <c:v>0.21</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>2.4300000000000002</c:v>
+                  <c:v>0.37</c:v>
                 </c:pt>
                 <c:pt idx="113">
                   <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>3.5</c:v>
+                  <c:v>3.3</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>4.7</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="116">
                   <c:v>6</c:v>
@@ -15579,13 +15579,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="117"/>
                 <c:pt idx="99">
-                  <c:v>0.63</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>2.79</c:v>
+                  <c:v>1.9</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>4.71</c:v>
+                  <c:v>3.2</c:v>
                 </c:pt>
                 <c:pt idx="102">
                   <c:v>4.71</c:v>
@@ -15603,34 +15603,34 @@
                   <c:v>4.71</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>4.1900000000000004</c:v>
+                  <c:v>3.8</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>3.32</c:v>
+                  <c:v>3.12</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>2.97</c:v>
+                  <c:v>2.4</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>3.3</c:v>
+                  <c:v>1.625</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>3.23</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>3.32</c:v>
+                  <c:v>0.86</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>3.49</c:v>
+                  <c:v>0.76</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>0.87</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>0.85</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>0.84</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -18726,31 +18726,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="117"/>
                 <c:pt idx="99">
-                  <c:v>25</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>25</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>25</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>25</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>23</c:v>
+                  <c:v>28.666667</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>21.7</c:v>
+                  <c:v>27.333333</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>20.100000000000001</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>18.899999999999999</c:v>
+                  <c:v>24.666667</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>17.399999999999999</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="108">
                   <c:v>17</c:v>
@@ -18759,25 +18759,25 @@
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>15</c:v>
+                  <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>13</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>12</c:v>
+                  <c:v>11.4</c:v>
                 </c:pt>
                 <c:pt idx="113">
                   <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="115">
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -21861,10 +21861,10 @@
                   <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>1.6</c:v>
+                  <c:v>1.57</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>1.6</c:v>
+                  <c:v>1.54</c:v>
                 </c:pt>
                 <c:pt idx="103">
                   <c:v>1.46</c:v>
@@ -21876,7 +21876,7 @@
                   <c:v>1.3</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>1.28</c:v>
+                  <c:v>1.23</c:v>
                 </c:pt>
                 <c:pt idx="107">
                   <c:v>1.1000000000000001</c:v>
@@ -21891,22 +21891,22 @@
                   <c:v>0.95</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>0.9</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="112">
                   <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>0.45</c:v>
+                  <c:v>0.52</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>0.37</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>0.3</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>0.2</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -26033,15 +26033,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>185737</xdr:colOff>
-      <xdr:row>119</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>63499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>642937</xdr:colOff>
-      <xdr:row>134</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>211667</xdr:colOff>
+      <xdr:row>139</xdr:row>
+      <xdr:rowOff>113768</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -26068,16 +26068,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>119</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>217488</xdr:colOff>
+      <xdr:row>123</xdr:row>
+      <xdr:rowOff>103186</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>134</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>484188</xdr:colOff>
+      <xdr:row>141</xdr:row>
+      <xdr:rowOff>21166</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -26104,16 +26104,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>120</xdr:row>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>465667</xdr:colOff>
+      <xdr:row>121</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>135</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>148166</xdr:colOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>21167</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -26140,16 +26140,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>120</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>179917</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>84667</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>135</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>518582</xdr:colOff>
+      <xdr:row>145</xdr:row>
+      <xdr:rowOff>52916</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -26584,8 +26584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD9B3CC4-9666-4EB6-BA6C-1D18D3C8D9BE}">
   <dimension ref="A1:BJ119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BD2" sqref="BD2:BJ119"/>
+    <sheetView tabSelected="1" topLeftCell="AR103" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AV119" sqref="AS118:AV119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -31123,37 +31123,37 @@
         <v>0</v>
       </c>
       <c r="G102">
-        <v>1.6500000000000001E-2</v>
+        <v>1.6299999999999999E-2</v>
       </c>
       <c r="K102">
         <v>0</v>
       </c>
       <c r="Q102">
-        <v>5.5E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="T102">
         <v>0</v>
       </c>
       <c r="Z102">
-        <v>0.19800000000000001</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="AC102">
         <v>0</v>
       </c>
       <c r="AI102">
-        <v>0.22</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="AL102">
         <v>0</v>
       </c>
       <c r="AR102">
-        <v>0.63</v>
+        <v>0.5</v>
       </c>
       <c r="AU102">
         <v>0</v>
       </c>
       <c r="BA102">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="BD102">
         <v>0</v>
@@ -31167,37 +31167,37 @@
         <v>0.2</v>
       </c>
       <c r="G103">
-        <v>1.6500000000000001E-2</v>
+        <v>1.6299999999999999E-2</v>
       </c>
       <c r="K103">
         <v>0.2</v>
       </c>
       <c r="Q103">
-        <v>5.5E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="T103">
         <v>0.2</v>
       </c>
       <c r="Z103">
-        <v>0.19800000000000001</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="AC103">
         <v>0.2</v>
       </c>
       <c r="AI103">
-        <v>0.22</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="AL103">
         <v>0.2</v>
       </c>
       <c r="AR103">
-        <v>2.79</v>
+        <v>1.9</v>
       </c>
       <c r="AU103">
         <v>0.2</v>
       </c>
       <c r="BA103">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="BD103">
         <v>0.2</v>
@@ -31211,43 +31211,43 @@
         <v>0.4</v>
       </c>
       <c r="G104">
-        <v>1.6500000000000001E-2</v>
+        <v>1.6299999999999999E-2</v>
       </c>
       <c r="K104">
         <v>0.4</v>
       </c>
       <c r="Q104">
-        <v>5.5E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="T104">
         <v>0.4</v>
       </c>
       <c r="Z104">
-        <v>0.19800000000000001</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="AC104">
         <v>0.4</v>
       </c>
       <c r="AI104">
-        <v>0.22</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="AL104">
         <v>0.4</v>
       </c>
       <c r="AR104">
-        <v>4.71</v>
+        <v>3.2</v>
       </c>
       <c r="AU104">
         <v>0.4</v>
       </c>
       <c r="BA104">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="BD104">
         <v>0.4</v>
       </c>
       <c r="BJ104">
-        <v>1.6</v>
+        <v>1.57</v>
       </c>
     </row>
     <row r="105" spans="1:62" x14ac:dyDescent="0.2">
@@ -31255,25 +31255,25 @@
         <v>0.6</v>
       </c>
       <c r="G105">
-        <v>1.7500000000000002E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="K105">
         <v>0.6</v>
       </c>
       <c r="Q105">
-        <v>5.5E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="T105">
         <v>0.6</v>
       </c>
       <c r="Z105">
-        <v>0.19800000000000001</v>
+        <v>0.128</v>
       </c>
       <c r="AC105">
         <v>0.6</v>
       </c>
       <c r="AI105">
-        <v>0.28000000000000003</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="AL105">
         <v>0.6</v>
@@ -31285,13 +31285,13 @@
         <v>0.6</v>
       </c>
       <c r="BA105">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="BD105">
         <v>0.6</v>
       </c>
       <c r="BJ105">
-        <v>1.6</v>
+        <v>1.54</v>
       </c>
     </row>
     <row r="106" spans="1:62" x14ac:dyDescent="0.2">
@@ -31299,25 +31299,25 @@
         <v>0.7</v>
       </c>
       <c r="G106">
-        <v>0.02</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="K106">
         <v>0.7</v>
       </c>
       <c r="Q106">
-        <v>5.5E-2</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="T106">
         <v>0.7</v>
       </c>
       <c r="Z106">
-        <v>0.19800000000000001</v>
+        <v>0.12</v>
       </c>
       <c r="AC106">
         <v>0.7</v>
       </c>
       <c r="AI106">
-        <v>0.28000000000000003</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="AL106">
         <v>0.7</v>
@@ -31329,7 +31329,7 @@
         <v>0.7</v>
       </c>
       <c r="BA106">
-        <v>23</v>
+        <v>28.666667</v>
       </c>
       <c r="BD106">
         <v>0.7</v>
@@ -31343,25 +31343,25 @@
         <v>0.8</v>
       </c>
       <c r="G107">
-        <v>0.02</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="K107">
         <v>0.8</v>
       </c>
       <c r="Q107">
-        <v>5.5E-2</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="T107">
         <v>0.8</v>
       </c>
       <c r="Z107">
-        <v>0.19800000000000001</v>
+        <v>0.123</v>
       </c>
       <c r="AC107">
         <v>0.8</v>
       </c>
       <c r="AI107">
-        <v>0.28000000000000003</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="AL107">
         <v>0.8</v>
@@ -31373,7 +31373,7 @@
         <v>0.8</v>
       </c>
       <c r="BA107">
-        <v>21.7</v>
+        <v>27.333333</v>
       </c>
       <c r="BD107">
         <v>0.8</v>
@@ -31387,25 +31387,25 @@
         <v>0.9</v>
       </c>
       <c r="G108">
-        <v>1.84E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="K108">
         <v>0.9</v>
       </c>
       <c r="Q108">
-        <v>5.8000000000000003E-2</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="T108">
         <v>0.9</v>
       </c>
       <c r="Z108">
-        <v>0.19800000000000001</v>
+        <v>0.155</v>
       </c>
       <c r="AC108">
         <v>0.9</v>
       </c>
       <c r="AI108">
-        <v>0.2</v>
+        <v>0.06</v>
       </c>
       <c r="AL108">
         <v>0.9</v>
@@ -31417,7 +31417,7 @@
         <v>0.9</v>
       </c>
       <c r="BA108">
-        <v>20.100000000000001</v>
+        <v>26</v>
       </c>
       <c r="BD108">
         <v>0.9</v>
@@ -31431,25 +31431,25 @@
         <v>1</v>
       </c>
       <c r="G109">
-        <v>1.7999999999999999E-2</v>
+        <v>0.03</v>
       </c>
       <c r="K109">
         <v>1</v>
       </c>
       <c r="Q109">
-        <v>6.2E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="T109">
         <v>1</v>
       </c>
       <c r="Z109">
-        <v>0.19800000000000001</v>
+        <v>0.18</v>
       </c>
       <c r="AC109">
         <v>1</v>
       </c>
       <c r="AI109">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="AL109">
         <v>1</v>
@@ -31461,13 +31461,13 @@
         <v>1</v>
       </c>
       <c r="BA109">
-        <v>18.899999999999999</v>
+        <v>24.666667</v>
       </c>
       <c r="BD109">
         <v>1</v>
       </c>
       <c r="BJ109">
-        <v>1.28</v>
+        <v>1.23</v>
       </c>
     </row>
     <row r="110" spans="1:62" x14ac:dyDescent="0.2">
@@ -31475,13 +31475,13 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="G110">
-        <v>1.9E-2</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="K110">
         <v>1.1000000000000001</v>
       </c>
       <c r="Q110">
-        <v>6.2E-2</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="T110">
         <v>1.1000000000000001</v>
@@ -31499,13 +31499,13 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="AR110">
-        <v>4.1900000000000004</v>
+        <v>3.8</v>
       </c>
       <c r="AU110">
         <v>1.1000000000000001</v>
       </c>
       <c r="BA110">
-        <v>17.399999999999999</v>
+        <v>18</v>
       </c>
       <c r="BD110">
         <v>1.1000000000000001</v>
@@ -31519,13 +31519,13 @@
         <v>1.2</v>
       </c>
       <c r="G111">
-        <v>2.1000000000000001E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="K111">
         <v>1.2</v>
       </c>
       <c r="Q111">
-        <v>6.2E-2</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="T111">
         <v>1.2</v>
@@ -31537,13 +31537,13 @@
         <v>1.2</v>
       </c>
       <c r="AI111">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="AL111">
         <v>1.2</v>
       </c>
       <c r="AR111">
-        <v>3.32</v>
+        <v>3.12</v>
       </c>
       <c r="AU111">
         <v>1.2</v>
@@ -31563,13 +31563,13 @@
         <v>1.3</v>
       </c>
       <c r="G112">
-        <v>2.1000000000000001E-2</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="K112">
         <v>1.3</v>
       </c>
       <c r="Q112">
-        <v>0.06</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="T112">
         <v>1.3</v>
@@ -31581,13 +31581,13 @@
         <v>1.3</v>
       </c>
       <c r="AI112">
-        <v>0.1</v>
+        <v>0.96</v>
       </c>
       <c r="AL112">
         <v>1.3</v>
       </c>
       <c r="AR112">
-        <v>2.97</v>
+        <v>2.4</v>
       </c>
       <c r="AU112">
         <v>1.3</v>
@@ -31607,13 +31607,13 @@
         <v>1.4</v>
       </c>
       <c r="G113">
-        <v>2.0500000000000001E-2</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="K113">
         <v>1.4</v>
       </c>
       <c r="Q113">
-        <v>5.6000000000000001E-2</v>
+        <v>6.9500000000000006E-2</v>
       </c>
       <c r="T113">
         <v>1.4</v>
@@ -31631,13 +31631,13 @@
         <v>1.4</v>
       </c>
       <c r="AR113">
-        <v>3.3</v>
+        <v>1.625</v>
       </c>
       <c r="AU113">
         <v>1.4</v>
       </c>
       <c r="BA113">
-        <v>15</v>
+        <v>14.5</v>
       </c>
       <c r="BD113">
         <v>1.4</v>
@@ -31651,13 +31651,13 @@
         <v>1.6</v>
       </c>
       <c r="G114">
-        <v>1.9E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="K114">
         <v>1.6</v>
       </c>
       <c r="Q114">
-        <v>5.1999999999999998E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="T114">
         <v>1.6</v>
@@ -31675,19 +31675,19 @@
         <v>1.6</v>
       </c>
       <c r="AR114">
-        <v>3.23</v>
+        <v>1.2</v>
       </c>
       <c r="AU114">
         <v>1.6</v>
       </c>
       <c r="BA114">
-        <v>13</v>
+        <v>12.5</v>
       </c>
       <c r="BD114">
         <v>1.6</v>
       </c>
       <c r="BJ114">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="115" spans="1:62" x14ac:dyDescent="0.2">
@@ -31695,13 +31695,13 @@
         <v>1.8</v>
       </c>
       <c r="G115">
-        <v>1.8599999999999998E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="K115">
         <v>1.8</v>
       </c>
       <c r="Q115">
-        <v>4.2000000000000003E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="T115">
         <v>1.8</v>
@@ -31713,19 +31713,19 @@
         <v>1.8</v>
       </c>
       <c r="AI115">
-        <v>2.4300000000000002</v>
+        <v>0.37</v>
       </c>
       <c r="AL115">
         <v>1.8</v>
       </c>
       <c r="AR115">
-        <v>3.32</v>
+        <v>0.86</v>
       </c>
       <c r="AU115">
         <v>1.8</v>
       </c>
       <c r="BA115">
-        <v>12</v>
+        <v>11.4</v>
       </c>
       <c r="BD115">
         <v>1.8</v>
@@ -31739,7 +31739,7 @@
         <v>2</v>
       </c>
       <c r="G116">
-        <v>1.8599999999999998E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="K116">
         <v>2</v>
@@ -31763,7 +31763,7 @@
         <v>2</v>
       </c>
       <c r="AR116">
-        <v>3.49</v>
+        <v>0.76</v>
       </c>
       <c r="AU116">
         <v>2</v>
@@ -31775,7 +31775,7 @@
         <v>2</v>
       </c>
       <c r="BJ116">
-        <v>0.45</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="117" spans="1:62" x14ac:dyDescent="0.2">
@@ -31783,13 +31783,13 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="G117">
-        <v>1.8599999999999998E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="K117">
         <v>2.2000000000000002</v>
       </c>
       <c r="Q117">
-        <v>3.6999999999999998E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T117">
         <v>2.2000000000000002</v>
@@ -31801,25 +31801,25 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="AI117">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="AL117">
         <v>2.2000000000000002</v>
       </c>
       <c r="AR117">
-        <v>0.87</v>
+        <v>0.7</v>
       </c>
       <c r="AU117">
         <v>2.2000000000000002</v>
       </c>
       <c r="BA117">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="BD117">
         <v>2.2000000000000002</v>
       </c>
       <c r="BJ117">
-        <v>0.37</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="118" spans="1:62" x14ac:dyDescent="0.2">
@@ -31827,7 +31827,7 @@
         <v>2.5</v>
       </c>
       <c r="G118">
-        <v>1.7999999999999999E-2</v>
+        <v>3.9E-2</v>
       </c>
       <c r="K118">
         <v>2.5</v>
@@ -31845,13 +31845,13 @@
         <v>2.5</v>
       </c>
       <c r="AI118">
-        <v>4.7</v>
+        <v>4.5</v>
       </c>
       <c r="AL118">
         <v>2.5</v>
       </c>
       <c r="AR118">
-        <v>0.85</v>
+        <v>0.7</v>
       </c>
       <c r="AU118">
         <v>2.5</v>
@@ -31863,7 +31863,7 @@
         <v>2.5</v>
       </c>
       <c r="BJ118">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="119" spans="1:62" x14ac:dyDescent="0.2">
@@ -31871,13 +31871,13 @@
         <v>3.9</v>
       </c>
       <c r="G119">
-        <v>2.1999999999999999E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="K119">
         <v>3.9</v>
       </c>
       <c r="Q119">
-        <v>2.3E-2</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="T119">
         <v>3.9</v>
@@ -31895,19 +31895,19 @@
         <v>3.9</v>
       </c>
       <c r="AR119">
-        <v>0.84</v>
+        <v>0.7</v>
       </c>
       <c r="AU119">
         <v>3.9</v>
       </c>
       <c r="BA119">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="BD119">
         <v>3.9</v>
       </c>
       <c r="BJ119">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>